<commit_message>
Top servo housing and uprights adjusted
</commit_message>
<xml_diff>
--- a/Parts List.xlsx
+++ b/Parts List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uctcloud-my.sharepoint.com/personal/kdrabd004_myuct_ac_za/Documents/Varsity Work/2025 (4th Year)/EEE4113F/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uctcloud-my.sharepoint.com/personal/kdrabd004_myuct_ac_za/Documents/Varsity Work/2025 (4th Year)/EEE4113F/EEE4113F-Group-1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="101_S{67755801-AC3A-547C-9AA1-881D8B3CA615}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A526BB30-425C-4641-9A1C-2F0C3265D670}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="101_S{67755801-AC3A-547C-9AA1-881D8B3CA615}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{37E149B6-8FAC-48E3-82E3-AB8DB6844993}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16340" xr2:uid="{0FD2535E-9E40-4B61-9F93-D9E091BB756B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{0FD2535E-9E40-4B61-9F93-D9E091BB756B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -452,6 +452,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -459,12 +465,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -483,10 +483,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -808,21 +804,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A425CD9F-5F71-4DC4-AE29-D4E58D3C41E0}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F5"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="20" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="20" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="28" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="52.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="52.44140625" style="1" customWidth="1"/>
     <col min="3" max="5" width="20" style="1"/>
     <col min="6" max="6" width="88.33203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="74.33203125" style="1" customWidth="1"/>
     <col min="8" max="16384" width="20" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
@@ -842,8 +838,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="33" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="35" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -863,8 +859,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A3" s="34"/>
+    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="36"/>
       <c r="B3" s="26" t="s">
         <v>8</v>
       </c>
@@ -875,15 +871,15 @@
         <v>1</v>
       </c>
       <c r="E3" s="10">
-        <f t="shared" ref="E3:E10" si="0">(C3*D3)</f>
+        <f t="shared" ref="E3:E9" si="0">(C3*D3)</f>
         <v>394.45</v>
       </c>
       <c r="F3" s="16" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="34"/>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="36"/>
       <c r="B4" s="27" t="s">
         <v>10</v>
       </c>
@@ -901,8 +897,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="34"/>
+    <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="36"/>
       <c r="B5" s="3" t="s">
         <v>12</v>
       </c>
@@ -920,7 +916,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="29" t="s">
         <v>14</v>
       </c>
@@ -941,8 +937,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="34" t="s">
+    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="36" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -951,7 +947,7 @@
       <c r="C7" s="25">
         <v>99</v>
       </c>
-      <c r="D7" s="37">
+      <c r="D7" s="34">
         <v>1</v>
       </c>
       <c r="E7" s="19">
@@ -962,46 +958,46 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="34"/>
+    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="36"/>
       <c r="B8" s="3" t="s">
         <v>29</v>
       </c>
       <c r="C8" s="25">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="D8" s="14">
         <v>2</v>
       </c>
-      <c r="E8" s="36">
+      <c r="E8" s="33">
         <f>(C8*D8)</f>
-        <v>26</v>
+        <v>86</v>
       </c>
       <c r="F8" s="16" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="34"/>
+    <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="36"/>
       <c r="B9" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C9" s="25">
-        <v>95</v>
+        <v>55</v>
       </c>
       <c r="D9" s="14">
         <v>2</v>
       </c>
       <c r="E9" s="10">
         <f t="shared" si="0"/>
-        <v>190</v>
+        <v>110</v>
       </c>
       <c r="F9" s="16" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="35"/>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="37"/>
       <c r="B10" s="4" t="s">
         <v>22</v>
       </c>
@@ -1019,21 +1015,21 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D11" s="6" t="s">
         <v>4</v>
       </c>
       <c r="E11" s="18">
         <f>SUM(E2:E10)</f>
-        <v>1400.35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+        <v>1380.35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" ht="15" x14ac:dyDescent="0.35">
       <c r="A17" s="21" t="s">
         <v>24</v>
       </c>
@@ -1041,7 +1037,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="46" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" ht="70.2" x14ac:dyDescent="0.5">
       <c r="A18" s="22" t="s">
         <v>26</v>
       </c>
@@ -1049,7 +1045,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" ht="15" x14ac:dyDescent="0.35">
       <c r="A19" s="21" t="s">
         <v>15</v>
       </c>
@@ -1080,12 +1076,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="5e3dcce6-8d7a-4a97-bc3c-0c26ec5308c1" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1336,17 +1331,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="5e3dcce6-8d7a-4a97-bc3c-0c26ec5308c1" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21B835A0-3332-4856-8E57-25BDD5F8A2DE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A23AEE34-1C37-4A9B-87A2-9AA35BBB5357}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="5e3dcce6-8d7a-4a97-bc3c-0c26ec5308c1"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="e45d0e85-392f-4e41-9dfa-b4bf94b9865e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1371,18 +1376,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A23AEE34-1C37-4A9B-87A2-9AA35BBB5357}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21B835A0-3332-4856-8E57-25BDD5F8A2DE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="5e3dcce6-8d7a-4a97-bc3c-0c26ec5308c1"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="e45d0e85-392f-4e41-9dfa-b4bf94b9865e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>